<commit_message>
commit tmp kwitansi & spby
</commit_message>
<xml_diff>
--- a/report/KWITANSI.xlsx
+++ b/report/KWITANSI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/simontok/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF70840-CD7A-2944-A113-DA4BBBE6EB76}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D036F89-CF96-B84E-81B9-059A3694F7B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="27320" windowHeight="13820" xr2:uid="{70B685DE-DC4F-8041-8D6D-A6362B0E24DA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -33,9 +33,6 @@
     <t>T.A.</t>
   </si>
   <si>
-    <t>: 2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">     </t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Guna Membayar</t>
   </si>
   <si>
-    <t xml:space="preserve">Biaya pembelian konsumsi dalam rangka kegiatan Open House acara Halal Bi Halal Hari Raya Idul Fitri 1 Syawal 1439 H Direktorat Poltekkes Kemenkes Semarang pada tanggal 21 Juni 2018 dengan perincian sbb: </t>
-  </si>
-  <si>
     <t>Setuju dibayar :</t>
   </si>
   <si>
@@ -87,22 +81,10 @@
     <t>Penerima,</t>
   </si>
   <si>
-    <t>Marsum, BE, SPd. MHP.</t>
-  </si>
-  <si>
-    <t>NIP. 19630727 198403 1 001</t>
-  </si>
-  <si>
     <t>Lunas dibayar :</t>
   </si>
   <si>
     <t>Bendahara Pengeluaran</t>
-  </si>
-  <si>
-    <t>Wahyu Dwi Nuryanti, AMd.</t>
-  </si>
-  <si>
-    <t>NIP. 198612042014022002</t>
   </si>
   <si>
     <t>Pekerjaan tersebut telah diselesaikan dengan baik</t>
@@ -550,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DA878F-89B2-0C49-B0D2-A3906CE9B839}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -600,17 +582,17 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -623,10 +605,10 @@
       <c r="G4" s="2"/>
       <c r="H4" s="1"/>
       <c r="I4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -643,7 +625,7 @@
     </row>
     <row r="6" spans="1:10" ht="23" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -669,14 +651,14 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
@@ -687,11 +669,11 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="7"/>
@@ -703,11 +685,11 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -719,15 +701,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>14</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -845,7 +825,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -859,7 +839,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -868,14 +848,14 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -884,7 +864,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="3"/>
@@ -938,9 +918,7 @@
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="A28" s="13"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -952,9 +930,7 @@
       <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -990,7 +966,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1004,7 +980,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1018,7 +994,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1079,9 +1055,7 @@
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1093,9 +1067,7 @@
       <c r="J39" s="3"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1120,7 +1092,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -1182,7 +1154,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>

</xml_diff>